<commit_message>
modified code for highlighting primary keys
</commit_message>
<xml_diff>
--- a/src/main/resources/Reportsheet/Book1.xlsx
+++ b/src/main/resources/Reportsheet/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manju\IdeaProjects\filecomparision\src\main\resources\Reportsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71A3D77-21F2-4C50-A0CD-81582406EDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0E183D-74E1-4C91-9CF1-4AAA89CCDDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0184327C-E070-46EE-AF30-BEB50419C72F}"/>
+    <workbookView xWindow="3612" yWindow="1704" windowWidth="17280" windowHeight="8880" xr2:uid="{0184327C-E070-46EE-AF30-BEB50419C72F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t>Serial</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>TradeID</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -430,7 +439,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,7 +486,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -497,7 +506,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -517,7 +526,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -537,7 +546,7 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
included code for comparing primary key values
</commit_message>
<xml_diff>
--- a/src/main/resources/Reportsheet/Book1.xlsx
+++ b/src/main/resources/Reportsheet/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manju\IdeaProjects\filecomparision\src\main\resources\Reportsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11B97AE-8274-4AE9-BDF4-CB5D1DA68363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03A62B4-6AD9-446D-9D36-692B92731AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3612" yWindow="1704" windowWidth="17280" windowHeight="8880" xr2:uid="{0184327C-E070-46EE-AF30-BEB50419C72F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Serial</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>High</t>
-  </si>
-  <si>
-    <t>low</t>
   </si>
 </sst>
 </file>
@@ -523,7 +520,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>